<commit_message>
simulations partielles + intégration f1 score + ROC-AUC
simulations partielles + intégration f1 score + ROC-AUC
</commit_message>
<xml_diff>
--- a/docs/simutations-results.xlsx
+++ b/docs/simutations-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\bootcamp-mle24-rakuten\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A867F0-6B04-4430-A18F-8EE5A3E126DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BD9151-142E-4872-9842-AB661A060BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11700" yWindow="2475" windowWidth="22725" windowHeight="16905" xr2:uid="{129726B2-C076-44EF-86B9-B94A75B693D3}"/>
   </bookViews>
@@ -274,9 +274,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,6 +287,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -629,7 +629,7 @@
   <dimension ref="B1:AE32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,126 +647,126 @@
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
     </row>
     <row r="3" spans="2:30" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>10</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>40</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>50</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <v>60</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="16">
         <v>1140</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="16">
         <v>1160</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="16">
         <v>1180</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="16">
         <v>1280</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="16">
         <v>1281</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="16">
         <v>1300</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="16">
         <v>1301</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="16">
         <v>1302</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="16">
         <v>1320</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="16">
         <v>1560</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="Q3" s="16">
         <v>1920</v>
       </c>
-      <c r="R3" s="17">
+      <c r="R3" s="16">
         <v>1940</v>
       </c>
-      <c r="S3" s="17">
+      <c r="S3" s="16">
         <v>2060</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="16">
         <v>2220</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="16">
         <v>2280</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="16">
         <v>2403</v>
       </c>
-      <c r="W3" s="17">
+      <c r="W3" s="16">
         <v>2462</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="16">
         <v>2522</v>
       </c>
-      <c r="Y3" s="17">
+      <c r="Y3" s="16">
         <v>2582</v>
       </c>
-      <c r="Z3" s="17">
+      <c r="Z3" s="16">
         <v>2583</v>
       </c>
-      <c r="AA3" s="17">
+      <c r="AA3" s="16">
         <v>2585</v>
       </c>
-      <c r="AB3" s="17">
+      <c r="AB3" s="16">
         <v>2705</v>
       </c>
-      <c r="AC3" s="19">
+      <c r="AC3" s="18">
         <v>2905</v>
       </c>
-      <c r="AD3" s="20" t="s">
+      <c r="AD3" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>10</v>
       </c>
       <c r="C4" s="5">
@@ -856,7 +856,7 @@
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>40</v>
       </c>
       <c r="C5" s="1">
@@ -946,7 +946,7 @@
       </c>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>50</v>
       </c>
       <c r="C6" s="1">
@@ -1036,7 +1036,7 @@
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>60</v>
       </c>
       <c r="C7" s="1">
@@ -1126,7 +1126,7 @@
       </c>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>1140</v>
       </c>
       <c r="C8" s="1">
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>1160</v>
       </c>
       <c r="C9" s="1">
@@ -1306,7 +1306,7 @@
       </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>1180</v>
       </c>
       <c r="C10" s="1">
@@ -1396,7 +1396,7 @@
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>1280</v>
       </c>
       <c r="C11" s="1">
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>1281</v>
       </c>
       <c r="C12" s="1">
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>1300</v>
       </c>
       <c r="C13" s="1">
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>1301</v>
       </c>
       <c r="C14" s="1">
@@ -1754,7 +1754,7 @@
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>1302</v>
       </c>
       <c r="C15" s="1">
@@ -1844,7 +1844,7 @@
       </c>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>1320</v>
       </c>
       <c r="C16" s="1">
@@ -1934,7 +1934,7 @@
       </c>
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>1560</v>
       </c>
       <c r="C17" s="1">
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>1920</v>
       </c>
       <c r="C18" s="1">
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>1940</v>
       </c>
       <c r="C19" s="1">
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="17">
+      <c r="B20" s="16">
         <v>2060</v>
       </c>
       <c r="C20" s="1">
@@ -2294,7 +2294,7 @@
       </c>
     </row>
     <row r="21" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <v>2220</v>
       </c>
       <c r="C21" s="1">
@@ -2384,7 +2384,7 @@
       </c>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <v>2280</v>
       </c>
       <c r="C22" s="1">
@@ -2474,7 +2474,7 @@
       </c>
     </row>
     <row r="23" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>2403</v>
       </c>
       <c r="C23" s="1">
@@ -2564,7 +2564,7 @@
       </c>
     </row>
     <row r="24" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B24" s="17">
+      <c r="B24" s="16">
         <v>2462</v>
       </c>
       <c r="C24" s="1">
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="25" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>2522</v>
       </c>
       <c r="C25" s="1">
@@ -2744,7 +2744,7 @@
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>2582</v>
       </c>
       <c r="C26" s="1">
@@ -2834,7 +2834,7 @@
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>2583</v>
       </c>
       <c r="C27" s="1">
@@ -2924,7 +2924,7 @@
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B28" s="17">
+      <c r="B28" s="16">
         <v>2585</v>
       </c>
       <c r="C28" s="1">
@@ -3014,7 +3014,7 @@
       </c>
     </row>
     <row r="29" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>2705</v>
       </c>
       <c r="C29" s="1">
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="30" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B30" s="17">
+      <c r="B30" s="16">
         <v>2905</v>
       </c>
       <c r="C30" s="1">
@@ -3194,7 +3194,7 @@
       </c>
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="8">
@@ -3233,7 +3233,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="14">
         <f>1-L13/SUM(L4:L30)</f>
         <v>0.71531791907514453</v>
       </c>
@@ -3273,7 +3273,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V31" s="15">
+      <c r="V31" s="14">
         <f>1-V23/SUM(V4:V30)</f>
         <v>5.7409879839786404E-2</v>
       </c>
@@ -3309,7 +3309,7 @@
         <f>SUM(AD4:AD30)</f>
         <v>16453</v>
       </c>
-      <c r="AE31" s="16" t="s">
+      <c r="AE31" s="15" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>